<commit_message>
decided on prelim data normalisation
</commit_message>
<xml_diff>
--- a/development/datasets/order_data_normalisation.xlsx
+++ b/development/datasets/order_data_normalisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevan\Documents\jupyter\smu\smu_fyp\DemandPrediction\CloudWine_DemandPrediction\development\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346F3443-2B9E-4A1E-B3DC-FC0818AA7AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3836D5-1E3E-4F99-AE91-D6675324A07E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,23 +25,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Original Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>New Name</t>
   </si>
   <si>
     <t>Normalisation</t>
+  </si>
+  <si>
+    <t>Original Column Name</t>
+  </si>
+  <si>
+    <t>KIV</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Risk Level</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Billing Province Name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Created at</t>
+  </si>
+  <si>
+    <t>Lineitem quantity</t>
+  </si>
+  <si>
+    <t>Lineitem name</t>
+  </si>
+  <si>
+    <t>Lineitem price</t>
+  </si>
+  <si>
+    <t>Lineitem discount</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>remove the hashtags and enumerate from 0</t>
+  </si>
+  <si>
+    <t>order_time</t>
+  </si>
+  <si>
+    <t>item_price</t>
+  </si>
+  <si>
+    <t>item_quantity</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>standardise from 0 to 1</t>
+  </si>
+  <si>
+    <t>join with product data and the convert to their IDs</t>
+  </si>
+  <si>
+    <t>change to percentage in reference to nominal item price. Then bin them to categories to interval of 20%</t>
+  </si>
+  <si>
+    <t>item_discount_sub_twenty</t>
+  </si>
+  <si>
+    <t>item_discount_sub_forty</t>
+  </si>
+  <si>
+    <t>item_discount_sub_sixty</t>
+  </si>
+  <si>
+    <t>item_discount_sub_eighty</t>
+  </si>
+  <si>
+    <t>item_discount_sub_hundred</t>
+  </si>
+  <si>
+    <t>item_discount_null</t>
+  </si>
+  <si>
+    <t>item_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,28 +447,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>